<commit_message>
Added win screen and a few more boxs
</commit_message>
<xml_diff>
--- a/10 Credit Assesment (Game)/Game Testing Log.xlsx
+++ b/10 Credit Assesment (Game)/Game Testing Log.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raeffe.mccabe\OneDrive - Southland Boys' High School\DTC Level 1\10 Credit Assesment (Game)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFBCFCA-2B32-4C61-839B-8DCD6C1DB68E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{52417D2C-423C-4996-AD48-34911EA45B0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A4740EA8-4B8B-4BE0-B10F-2A8FE17358D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>What is being tested</t>
   </si>
@@ -57,6 +57,9 @@
     <t>playerXpos decreases and player image moves left on canvas</t>
   </si>
   <si>
+    <t>playerXpos decreases and player image moves left on canvas.</t>
+  </si>
+  <si>
     <t>moving Right</t>
   </si>
   <si>
@@ -66,20 +69,71 @@
     <t>PlayerXpos Increases and PlayerImage moves right on Canvas</t>
   </si>
   <si>
+    <t>PlayerXpos Increases and PlayerImage moves right on Canvas.</t>
+  </si>
+  <si>
+    <t>Jumping Up</t>
+  </si>
+  <si>
+    <t>Up arrow key</t>
+  </si>
+  <si>
     <t>PlayerYpos Increases  and player image also shifts up but then needs to wait 1 sec to go up the canvas do again</t>
   </si>
   <si>
-    <t>Jumping Up</t>
-  </si>
-  <si>
-    <t>Up arrow key</t>
+    <t>PlayerYpos Increases  and player image also shifts up but then needs to wait 1 sec to go up the canvas do again.</t>
+  </si>
+  <si>
+    <t>Contact with box</t>
+  </si>
+  <si>
+    <t>any arrow key</t>
+  </si>
+  <si>
+    <t>Box should cause the players pos to move a different way to create the illusion of a collision</t>
+  </si>
+  <si>
+    <t>Box should cause the players pos to move a different way to create the illusion of a collision.</t>
+  </si>
+  <si>
+    <t>Contact with Heart</t>
+  </si>
+  <si>
+    <t>When in contact with Heart area the Winning screen coshould me up displaying the name and "Congrats"</t>
+  </si>
+  <si>
+    <t>When in contact with Heart area the Winning screen coshould me up displaying the name and "Congrats".</t>
+  </si>
+  <si>
+    <t>Gravity</t>
+  </si>
+  <si>
+    <t>Not moving</t>
+  </si>
+  <si>
+    <t>When PLAYER_SIZE past the canvas width or height black death screen should come up displaying player name and "Nice try"</t>
+  </si>
+  <si>
+    <t>When PLAYER_SIZE past the canvas width or height black death screen should come up displaying player name and "Nice try".</t>
+  </si>
+  <si>
+    <t>Spawn</t>
+  </si>
+  <si>
+    <t>Start game</t>
+  </si>
+  <si>
+    <t>Player starting pos should be to the right of the map at the start</t>
+  </si>
+  <si>
+    <t>Player starting pos should be to the right of the map at the start.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,10 +527,10 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="36.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" style="1" customWidth="1"/>
@@ -484,7 +538,7 @@
     <col min="4" max="4" width="53.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -498,7 +552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="33.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -508,135 +562,173 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="33">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="49.5">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="33">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="49.5">
+      <c r="A10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="49.5">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="33">
+      <c r="A14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -649,6 +741,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100130DF9D54857EF409A9FC18598A3407A" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="94e9ad61f1eee94569bd3bd2f4985a0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="af4d1c43-0c8e-4afc-87fa-06d6eb99ec6b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ab77b9c0a1d65f498ed1a99564b02cc0" ns2:_="">
     <xsd:import namespace="af4d1c43-0c8e-4afc-87fa-06d6eb99ec6b"/>
@@ -800,15 +901,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -818,37 +910,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A8DCE70-9A99-4820-8203-E4AF4B0642B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="af4d1c43-0c8e-4afc-87fa-06d6eb99ec6b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E60CF964-E5B0-4456-94C9-62848076981E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E60CF964-E5B0-4456-94C9-62848076981E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A8DCE70-9A99-4820-8203-E4AF4B0642B7}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49705E9F-1DBC-44ED-AB34-BAD166CF391C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="af4d1c43-0c8e-4afc-87fa-06d6eb99ec6b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49705E9F-1DBC-44ED-AB34-BAD166CF391C}"/>
 </file>
</xml_diff>